<commit_message>
Switch Board Layout finished, needs text and logo
</commit_message>
<xml_diff>
--- a/src/schematics/Ard_Shield/Gerber/ScouseTom_New_BOM.xlsx
+++ b/src/schematics/Ard_Shield/Gerber/ScouseTom_New_BOM.xlsx
@@ -404,7 +404,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -545,6 +545,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF333333"/>
+      <name val="Verdana"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="33">
@@ -888,7 +894,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -901,6 +907,7 @@
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1249,9 +1256,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G59" sqref="G59"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H32" sqref="H32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2205,7 +2212,7 @@
         <v>55</v>
       </c>
       <c r="G37" s="3">
-        <v>1464325</v>
+        <v>1438441</v>
       </c>
       <c r="H37" s="3"/>
     </row>
@@ -2536,8 +2543,8 @@
       <c r="F50" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="G50" s="3">
-        <v>1701256</v>
+      <c r="G50" s="6">
+        <v>2102522</v>
       </c>
       <c r="H50" s="3"/>
     </row>

</xml_diff>

<commit_message>
Added calculation of number of parts needed to order. I hate excel
</commit_message>
<xml_diff>
--- a/src/schematics/Ard_Shield/Gerber/ScouseTom_New_BOM.xlsx
+++ b/src/schematics/Ard_Shield/Gerber/ScouseTom_New_BOM.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jimbles\Copy\ScouseTom\src\schematics\Ard_Shield\Gerber\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="480" yWindow="75" windowWidth="15315" windowHeight="25845"/>
   </bookViews>
@@ -12,7 +17,7 @@
   <definedNames>
     <definedName name="ScouseTom_New" localSheetId="0">Sheet1!$A$1:$H$52</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -41,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="121">
   <si>
     <t>Part</t>
   </si>
@@ -398,13 +403,19 @@
   </si>
   <si>
     <t>Total</t>
+  </si>
+  <si>
+    <t>uniq</t>
+  </si>
+  <si>
+    <t>cnt non free</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="20" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -551,6 +562,12 @@
       <color rgb="FF333333"/>
       <name val="Verdana"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF222426"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="33">
@@ -894,7 +911,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -908,6 +925,10 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -953,11 +974,20 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.14996795556505021"/>
+      </font>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1010,7 +1040,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1045,7 +1075,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1254,11 +1284,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H58"/>
+  <dimension ref="A1:K58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H32" sqref="H32"/>
+      <selection pane="bottomLeft" activeCell="K49" sqref="K49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1270,11 +1300,12 @@
     <col min="5" max="5" width="41" style="5" customWidth="1"/>
     <col min="6" max="6" width="27" style="5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15" style="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="5"/>
+    <col min="8" max="8" width="35.7109375" style="5" customWidth="1"/>
+    <col min="9" max="9" width="9.140625" style="5"/>
+    <col min="12" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1299,8 +1330,14 @@
       <c r="H1" s="1" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J1" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="K1" s="7" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>7</v>
       </c>
@@ -1325,8 +1362,16 @@
       <c r="H2" s="3" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J2" s="8">
+        <f t="array" ref="J2">INDEX($G$2:$G$52, MATCH(0, COUNTIF($J$1:J1, $G$2:$G$52), 0))</f>
+        <v>1759246</v>
+      </c>
+      <c r="K2">
+        <f>COUNTIFS($G$2:$G$75,J2,$H$2:$H$75,"")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>12</v>
       </c>
@@ -1351,8 +1396,16 @@
       <c r="H3" s="3" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J3" s="8">
+        <f t="array" ref="J3">INDEX($G$2:$G$52, MATCH(0, COUNTIF($J$1:J2, $G$2:$G$52), 0))</f>
+        <v>1759265</v>
+      </c>
+      <c r="K3">
+        <f t="shared" ref="K3:K31" si="0">COUNTIFS($G$2:$G$75,J3,$H$2:$H$75,"")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>13</v>
       </c>
@@ -1375,8 +1428,16 @@
         <v>2320852</v>
       </c>
       <c r="H4" s="3"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J4" s="8">
+        <f t="array" ref="J4">INDEX($G$2:$G$52, MATCH(0, COUNTIF($J$1:J3, $G$2:$G$52), 0))</f>
+        <v>2320852</v>
+      </c>
+      <c r="K4">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>15</v>
       </c>
@@ -1401,8 +1462,16 @@
       <c r="H5" s="3" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J5" s="8">
+        <f t="array" ref="J5">INDEX($G$2:$G$52, MATCH(0, COUNTIF($J$1:J4, $G$2:$G$52), 0))</f>
+        <v>2320827</v>
+      </c>
+      <c r="K5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>16</v>
       </c>
@@ -1427,8 +1496,16 @@
       <c r="H6" s="3" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J6" s="8">
+        <f t="array" ref="J6">INDEX($G$2:$G$52, MATCH(0, COUNTIF($J$1:J5, $G$2:$G$52), 0))</f>
+        <v>2102587</v>
+      </c>
+      <c r="K6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>17</v>
       </c>
@@ -1451,8 +1528,16 @@
         <v>2320852</v>
       </c>
       <c r="H7" s="3"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J7" s="8">
+        <f t="array" ref="J7">INDEX($G$2:$G$52, MATCH(0, COUNTIF($J$1:J6, $G$2:$G$52), 0))</f>
+        <v>1438441</v>
+      </c>
+      <c r="K7">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>18</v>
       </c>
@@ -1477,8 +1562,16 @@
       <c r="H8" s="3" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J8" s="8">
+        <f t="array" ref="J8">INDEX($G$2:$G$52, MATCH(0, COUNTIF($J$1:J7, $G$2:$G$52), 0))</f>
+        <v>2336831</v>
+      </c>
+      <c r="K8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>20</v>
       </c>
@@ -1503,8 +1596,16 @@
       <c r="H9" s="3" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J9" s="8">
+        <f t="array" ref="J9">INDEX($G$2:$G$52, MATCH(0, COUNTIF($J$1:J8, $G$2:$G$52), 0))</f>
+        <v>2336780</v>
+      </c>
+      <c r="K9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>21</v>
       </c>
@@ -1529,8 +1630,16 @@
       <c r="H10" s="3" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J10" s="8">
+        <f t="array" ref="J10">INDEX($G$2:$G$52, MATCH(0, COUNTIF($J$1:J9, $G$2:$G$52), 0))</f>
+        <v>2352451</v>
+      </c>
+      <c r="K10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>22</v>
       </c>
@@ -1555,8 +1664,16 @@
       <c r="H11" s="3" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J11" s="8">
+        <f t="array" ref="J11">INDEX($G$2:$G$52, MATCH(0, COUNTIF($J$1:J10, $G$2:$G$52), 0))</f>
+        <v>2129074</v>
+      </c>
+      <c r="K11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>23</v>
       </c>
@@ -1581,8 +1698,16 @@
       <c r="H12" s="3" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J12" s="8">
+        <f t="array" ref="J12">INDEX($G$2:$G$52, MATCH(0, COUNTIF($J$1:J11, $G$2:$G$52), 0))</f>
+        <v>9332391</v>
+      </c>
+      <c r="K12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>24</v>
       </c>
@@ -1605,8 +1730,16 @@
         <v>2320852</v>
       </c>
       <c r="H13" s="3"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J13" s="8">
+        <f t="array" ref="J13">INDEX($G$2:$G$52, MATCH(0, COUNTIF($J$1:J12, $G$2:$G$52), 0))</f>
+        <v>2129087</v>
+      </c>
+      <c r="K13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>25</v>
       </c>
@@ -1631,8 +1764,16 @@
       <c r="H14" s="3" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J14" s="8">
+        <f t="array" ref="J14">INDEX($G$2:$G$52, MATCH(0, COUNTIF($J$1:J13, $G$2:$G$52), 0))</f>
+        <v>2129237</v>
+      </c>
+      <c r="K14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>26</v>
       </c>
@@ -1655,8 +1796,16 @@
         <v>2320852</v>
       </c>
       <c r="H15" s="3"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J15" s="8">
+        <f t="array" ref="J15">INDEX($G$2:$G$52, MATCH(0, COUNTIF($J$1:J14, $G$2:$G$52), 0))</f>
+        <v>2129171</v>
+      </c>
+      <c r="K15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>27</v>
       </c>
@@ -1679,8 +1828,16 @@
         <v>2320852</v>
       </c>
       <c r="H16" s="3"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J16" s="8">
+        <f t="array" ref="J16">INDEX($G$2:$G$52, MATCH(0, COUNTIF($J$1:J15, $G$2:$G$52), 0))</f>
+        <v>2129150</v>
+      </c>
+      <c r="K16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>28</v>
       </c>
@@ -1705,8 +1862,16 @@
       <c r="H17" s="3" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J17" s="8">
+        <f t="array" ref="J17">INDEX($G$2:$G$52, MATCH(0, COUNTIF($J$1:J16, $G$2:$G$52), 0))</f>
+        <v>1838922</v>
+      </c>
+      <c r="K17">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>29</v>
       </c>
@@ -1731,8 +1896,16 @@
       <c r="H18" s="3" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J18" s="8">
+        <f t="array" ref="J18">INDEX($G$2:$G$52, MATCH(0, COUNTIF($J$1:J17, $G$2:$G$52), 0))</f>
+        <v>9425586</v>
+      </c>
+      <c r="K18">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>31</v>
       </c>
@@ -1757,8 +1930,16 @@
       <c r="H19" s="3" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J19" s="8">
+        <f t="array" ref="J19">INDEX($G$2:$G$52, MATCH(0, COUNTIF($J$1:J18, $G$2:$G$52), 0))</f>
+        <v>2102522</v>
+      </c>
+      <c r="K19">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>32</v>
       </c>
@@ -1783,8 +1964,16 @@
       <c r="H20" s="3" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J20" s="8">
+        <f t="array" ref="J20">INDEX($G$2:$G$52, MATCH(0, COUNTIF($J$1:J19, $G$2:$G$52), 0))</f>
+        <v>2067770</v>
+      </c>
+      <c r="K20">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>33</v>
       </c>
@@ -1809,8 +1998,16 @@
       <c r="H21" s="3" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J21" s="8" t="e">
+        <f t="array" ref="J21">INDEX($G$2:$G$52, MATCH(0, COUNTIF($J$1:J20, $G$2:$G$52), 0))</f>
+        <v>#N/A</v>
+      </c>
+      <c r="K21">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>34</v>
       </c>
@@ -1833,8 +2030,16 @@
         <v>2320852</v>
       </c>
       <c r="H22" s="3"/>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J22" s="8" t="e">
+        <f t="array" ref="J22">INDEX($G$2:$G$52, MATCH(0, COUNTIF($J$1:J21, $G$2:$G$52), 0))</f>
+        <v>#N/A</v>
+      </c>
+      <c r="K22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>35</v>
       </c>
@@ -1859,8 +2064,16 @@
       <c r="H23" s="3" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J23" s="8" t="e">
+        <f t="array" ref="J23">INDEX($G$2:$G$52, MATCH(0, COUNTIF($J$1:J22, $G$2:$G$52), 0))</f>
+        <v>#N/A</v>
+      </c>
+      <c r="K23">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>36</v>
       </c>
@@ -1885,8 +2098,16 @@
       <c r="H24" s="3" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J24" s="8" t="e">
+        <f t="array" ref="J24">INDEX($G$2:$G$52, MATCH(0, COUNTIF($J$1:J23, $G$2:$G$52), 0))</f>
+        <v>#N/A</v>
+      </c>
+      <c r="K24">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>37</v>
       </c>
@@ -1909,8 +2130,16 @@
         <v>2320852</v>
       </c>
       <c r="H25" s="3"/>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J25" s="8" t="e">
+        <f t="array" ref="J25">INDEX($G$2:$G$52, MATCH(0, COUNTIF($J$1:J24, $G$2:$G$52), 0))</f>
+        <v>#N/A</v>
+      </c>
+      <c r="K25">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>38</v>
       </c>
@@ -1935,8 +2164,16 @@
       <c r="H26" s="3" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J26" s="8" t="e">
+        <f t="array" ref="J26">INDEX($G$2:$G$52, MATCH(0, COUNTIF($J$1:J25, $G$2:$G$52), 0))</f>
+        <v>#N/A</v>
+      </c>
+      <c r="K26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>39</v>
       </c>
@@ -1961,8 +2198,16 @@
       <c r="H27" s="3" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J27" s="8" t="e">
+        <f t="array" ref="J27">INDEX($G$2:$G$52, MATCH(0, COUNTIF($J$1:J26, $G$2:$G$52), 0))</f>
+        <v>#N/A</v>
+      </c>
+      <c r="K27">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>40</v>
       </c>
@@ -1987,8 +2232,16 @@
       <c r="H28" s="3" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J28" s="8" t="e">
+        <f t="array" ref="J28">INDEX($G$2:$G$52, MATCH(0, COUNTIF($J$1:J27, $G$2:$G$52), 0))</f>
+        <v>#N/A</v>
+      </c>
+      <c r="K28">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>41</v>
       </c>
@@ -2011,8 +2264,16 @@
         <v>2320852</v>
       </c>
       <c r="H29" s="3"/>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J29" s="8" t="e">
+        <f t="array" ref="J29">INDEX($G$2:$G$52, MATCH(0, COUNTIF($J$1:J28, $G$2:$G$52), 0))</f>
+        <v>#N/A</v>
+      </c>
+      <c r="K29">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>42</v>
       </c>
@@ -2037,8 +2298,16 @@
       <c r="H30" s="3" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J30" s="8" t="e">
+        <f t="array" ref="J30">INDEX($G$2:$G$52, MATCH(0, COUNTIF($J$1:J29, $G$2:$G$52), 0))</f>
+        <v>#N/A</v>
+      </c>
+      <c r="K30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>43</v>
       </c>
@@ -2063,8 +2332,16 @@
       <c r="H31" s="3" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J31" s="8" t="e">
+        <f t="array" ref="J31">INDEX($G$2:$G$52, MATCH(0, COUNTIF($J$1:J30, $G$2:$G$52), 0))</f>
+        <v>#N/A</v>
+      </c>
+      <c r="K31">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>44</v>
       </c>
@@ -2087,8 +2364,12 @@
         <v>2320852</v>
       </c>
       <c r="H32" s="3"/>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J32" s="8" t="e">
+        <f t="array" ref="J32">INDEX($G$2:$G$52, MATCH(0, COUNTIF($J$1:J31, $G$2:$G$52), 0))</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>45</v>
       </c>
@@ -2113,8 +2394,12 @@
       <c r="H33" s="3" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J33" s="8" t="e">
+        <f t="array" ref="J33">INDEX($G$2:$G$52, MATCH(0, COUNTIF($J$1:J32, $G$2:$G$52), 0))</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>46</v>
       </c>
@@ -2139,8 +2424,12 @@
       <c r="H34" s="3" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J34" s="8" t="e">
+        <f t="array" ref="J34">INDEX($G$2:$G$52, MATCH(0, COUNTIF($J$1:J33, $G$2:$G$52), 0))</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
         <v>47</v>
       </c>
@@ -2165,8 +2454,12 @@
       <c r="H35" s="3" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J35" s="8" t="e">
+        <f t="array" ref="J35">INDEX($G$2:$G$52, MATCH(0, COUNTIF($J$1:J34, $G$2:$G$52), 0))</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>48</v>
       </c>
@@ -2191,8 +2484,12 @@
       <c r="H36" s="2" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J36" s="8" t="e">
+        <f t="array" ref="J36">INDEX($G$2:$G$52, MATCH(0, COUNTIF($J$1:J35, $G$2:$G$52), 0))</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
         <v>51</v>
       </c>
@@ -2215,8 +2512,12 @@
         <v>1438441</v>
       </c>
       <c r="H37" s="3"/>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J37" s="8" t="e">
+        <f t="array" ref="J37">INDEX($G$2:$G$52, MATCH(0, COUNTIF($J$1:J36, $G$2:$G$52), 0))</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
         <v>56</v>
       </c>
@@ -2241,8 +2542,12 @@
       <c r="H38" s="2" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J38" s="8" t="e">
+        <f t="array" ref="J38">INDEX($G$2:$G$52, MATCH(0, COUNTIF($J$1:J37, $G$2:$G$52), 0))</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
         <v>61</v>
       </c>
@@ -2267,8 +2572,12 @@
       <c r="H39" s="2" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J39" s="8" t="e">
+        <f t="array" ref="J39">INDEX($G$2:$G$52, MATCH(0, COUNTIF($J$1:J38, $G$2:$G$52), 0))</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
         <v>66</v>
       </c>
@@ -2293,8 +2602,12 @@
       <c r="H40" s="2" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J40" s="8" t="e">
+        <f t="array" ref="J40">INDEX($G$2:$G$52, MATCH(0, COUNTIF($J$1:J39, $G$2:$G$52), 0))</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
         <v>71</v>
       </c>
@@ -2319,8 +2632,12 @@
       <c r="H41" s="2" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J41" s="8" t="e">
+        <f t="array" ref="J41">INDEX($G$2:$G$52, MATCH(0, COUNTIF($J$1:J40, $G$2:$G$52), 0))</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
         <v>75</v>
       </c>
@@ -2345,8 +2662,12 @@
       <c r="H42" s="2" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J42" s="8" t="e">
+        <f t="array" ref="J42">INDEX($G$2:$G$52, MATCH(0, COUNTIF($J$1:J41, $G$2:$G$52), 0))</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
         <v>77</v>
       </c>
@@ -2371,8 +2692,12 @@
       <c r="H43" s="2" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J43" s="8" t="e">
+        <f t="array" ref="J43">INDEX($G$2:$G$52, MATCH(0, COUNTIF($J$1:J42, $G$2:$G$52), 0))</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
         <v>78</v>
       </c>
@@ -2397,8 +2722,12 @@
       <c r="H44" s="2" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J44" s="8" t="e">
+        <f t="array" ref="J44">INDEX($G$2:$G$52, MATCH(0, COUNTIF($J$1:J43, $G$2:$G$52), 0))</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
         <v>80</v>
       </c>
@@ -2423,8 +2752,12 @@
       <c r="H45" s="2" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J45" s="8" t="e">
+        <f t="array" ref="J45">INDEX($G$2:$G$52, MATCH(0, COUNTIF($J$1:J44, $G$2:$G$52), 0))</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
         <v>81</v>
       </c>
@@ -2449,8 +2782,12 @@
       <c r="H46" s="2" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J46" s="8" t="e">
+        <f t="array" ref="J46">INDEX($G$2:$G$52, MATCH(0, COUNTIF($J$1:J45, $G$2:$G$52), 0))</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
         <v>83</v>
       </c>
@@ -2475,8 +2812,12 @@
       <c r="H47" s="2" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J47" s="8" t="e">
+        <f t="array" ref="J47">INDEX($G$2:$G$52, MATCH(0, COUNTIF($J$1:J46, $G$2:$G$52), 0))</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
         <v>85</v>
       </c>
@@ -2499,8 +2840,12 @@
         <v>1838922</v>
       </c>
       <c r="H48" s="3"/>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J48" s="8" t="e">
+        <f t="array" ref="J48">INDEX($G$2:$G$52, MATCH(0, COUNTIF($J$1:J47, $G$2:$G$52), 0))</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
         <v>89</v>
       </c>
@@ -2523,8 +2868,12 @@
         <v>9425586</v>
       </c>
       <c r="H49" s="3"/>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J49" s="8" t="e">
+        <f t="array" ref="J49">INDEX($G$2:$G$52, MATCH(0, COUNTIF($J$1:J48, $G$2:$G$52), 0))</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
         <v>93</v>
       </c>
@@ -2548,7 +2897,7 @@
       </c>
       <c r="H50" s="3"/>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
         <v>96</v>
       </c>
@@ -2572,7 +2921,7 @@
       </c>
       <c r="H51" s="3"/>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
         <v>99</v>
       </c>
@@ -2596,7 +2945,7 @@
       </c>
       <c r="H52" s="3"/>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F55" s="3" t="s">
         <v>115</v>
       </c>
@@ -2605,7 +2954,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F56" s="3" t="s">
         <v>116</v>
       </c>
@@ -2614,7 +2963,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F57" s="3" t="s">
         <v>117</v>
       </c>
@@ -2623,7 +2972,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F58" s="3" t="s">
         <v>118</v>
       </c>
@@ -2633,6 +2982,11 @@
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="K1:K1048576">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Gerbers for updated shield, sent to PCBtrain. Minor edits to routing
</commit_message>
<xml_diff>
--- a/src/schematics/Ard_Shield/Gerber/ScouseTom_New_BOM.xlsx
+++ b/src/schematics/Ard_Shield/Gerber/ScouseTom_New_BOM.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jimbles\Copy\ScouseTom\src\schematics\Ard_Shield\Gerber\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jimbles\ScouseTom\src\schematics\Ard_Shield\Gerber\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="480" yWindow="75" windowWidth="15315" windowHeight="25845"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="BOM" sheetId="3" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="ScouseTom_New" localSheetId="0">Sheet1!$A$1:$H$52</definedName>
+    <definedName name="ScouseTom_New" localSheetId="0">BOM!$A$1:$G$56</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
 </workbook>
@@ -23,10 +23,9 @@
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" name="ScouseTom_New" type="6" refreshedVersion="4" background="1" saveData="1">
-    <textPr sourceFile="C:\Users\Jimbles\Copy\ScouseTom\src\schematics\Ard_Shield\ScouseTom_New.csv" tab="0" semicolon="1">
-      <textFields count="13">
-        <textField/>
+  <connection id="1" name="ScouseTom_New1" type="6" refreshedVersion="6" background="1" saveData="1">
+    <textPr sourceFile="C:\Users\Jimbles\ScouseTom\src\schematics\Ard_Shield\Gerber\ScouseTom_New.csv" tab="0" semicolon="1" consecutive="1">
+      <textFields count="12">
         <textField/>
         <textField/>
         <textField/>
@@ -46,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="125">
   <si>
     <t>Part</t>
   </si>
@@ -348,9 +347,6 @@
     <t>U5</t>
   </si>
   <si>
-    <t>TO-252</t>
-  </si>
-  <si>
     <t>LM317MDTX</t>
   </si>
   <si>
@@ -405,10 +401,25 @@
     <t>Total</t>
   </si>
   <si>
-    <t>uniq</t>
-  </si>
-  <si>
-    <t>cnt non free</t>
+    <t>DPACK</t>
+  </si>
+  <si>
+    <t>R8</t>
+  </si>
+  <si>
+    <t>R9</t>
+  </si>
+  <si>
+    <t>R10</t>
+  </si>
+  <si>
+    <t>R11</t>
+  </si>
+  <si>
+    <t>unique</t>
+  </si>
+  <si>
+    <t>non free stock to purchase</t>
   </si>
 </sst>
 </file>
@@ -911,7 +922,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -922,7 +933,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -994,7 +1004,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ScouseTom_New" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ScouseTom_New" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1284,1225 +1294,1239 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K58"/>
+  <dimension ref="A1:J62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K49" sqref="K49"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L21" sqref="L21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="41" style="5" customWidth="1"/>
-    <col min="6" max="6" width="27" style="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="35.7109375" style="5" customWidth="1"/>
-    <col min="9" max="9" width="9.140625" style="5"/>
-    <col min="12" max="16384" width="9.140625" style="5"/>
+    <col min="1" max="1" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="64.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="27" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="30.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="6" t="s">
         <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="J1" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="K1" s="7" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>7</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" s="3" t="s">
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" t="s">
         <v>11</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G2" s="2">
         <v>1759246</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="J2" s="8">
-        <f t="array" ref="J2">INDEX($G$2:$G$52, MATCH(0, COUNTIF($J$1:J1, $G$2:$G$52), 0))</f>
+        <v>103</v>
+      </c>
+      <c r="I2" s="7">
+        <f t="array" ref="I2">INDEX($G$2:$G$56, MATCH(0, COUNTIF(I$1:$J1, $G$2:$G$56), 0))</f>
         <v>1759246</v>
       </c>
-      <c r="K2">
-        <f>COUNTIFS($G$2:$G$75,J2,$H$2:$H$75,"")</f>
+      <c r="J2">
+        <f t="array" ref="J2">COUNTIFS($G$2:$G$57,I2,$H$2:$H$57,"")</f>
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>12</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" s="3" t="s">
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" t="s">
         <v>11</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G3" s="2">
         <v>1759265</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="J3" s="8">
-        <f t="array" ref="J3">INDEX($G$2:$G$52, MATCH(0, COUNTIF($J$1:J2, $G$2:$G$52), 0))</f>
+        <v>103</v>
+      </c>
+      <c r="I3" s="7">
+        <f t="array" ref="I3">INDEX($G$2:$G$56, MATCH(0, COUNTIF(I$1:$J2, $G$2:$G$56), 0))</f>
         <v>1759265</v>
       </c>
-      <c r="K3">
-        <f t="shared" ref="K3:K31" si="0">COUNTIFS($G$2:$G$75,J3,$H$2:$H$75,"")</f>
+      <c r="J3">
+        <f t="array" ref="J3">COUNTIFS($G$2:$G$57,I3,$H$2:$H$57,"")</f>
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>13</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" s="3" t="s">
+      <c r="C4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" t="s">
         <v>11</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G4" s="3">
         <v>2320852</v>
       </c>
       <c r="H4" s="3"/>
-      <c r="J4" s="8">
-        <f t="array" ref="J4">INDEX($G$2:$G$52, MATCH(0, COUNTIF($J$1:J3, $G$2:$G$52), 0))</f>
+      <c r="I4" s="7">
+        <f t="array" ref="I4">INDEX($G$2:$G$56, MATCH(0, COUNTIF(I$1:$J3, $G$2:$G$56), 0))</f>
         <v>2320852</v>
       </c>
-      <c r="K4">
-        <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+      <c r="J4">
+        <f t="array" ref="J4">COUNTIFS($G$2:$G$57,I4,$H$2:$H$57,"")</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>15</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5" s="3" t="s">
+      <c r="C5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" t="s">
         <v>11</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G5" s="2">
         <v>1759246</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="J5" s="8">
-        <f t="array" ref="J5">INDEX($G$2:$G$52, MATCH(0, COUNTIF($J$1:J4, $G$2:$G$52), 0))</f>
+        <v>103</v>
+      </c>
+      <c r="I5" s="7">
+        <f t="array" ref="I5">INDEX($G$2:$G$56, MATCH(0, COUNTIF(I$1:$J4, $G$2:$G$56), 0))</f>
         <v>2320827</v>
       </c>
-      <c r="K5">
-        <f t="shared" si="0"/>
+      <c r="J5">
+        <f t="array" ref="J5">COUNTIFS($G$2:$G$57,I5,$H$2:$H$57,"")</f>
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>16</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E6" s="3" t="s">
+      <c r="C6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" t="s">
         <v>11</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G6" s="2">
         <v>1759265</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="J6" s="8">
-        <f t="array" ref="J6">INDEX($G$2:$G$52, MATCH(0, COUNTIF($J$1:J5, $G$2:$G$52), 0))</f>
+        <v>103</v>
+      </c>
+      <c r="I6" s="7">
+        <f t="array" ref="I6">INDEX($G$2:$G$56, MATCH(0, COUNTIF(I$1:$J5, $G$2:$G$56), 0))</f>
         <v>2102587</v>
       </c>
-      <c r="K6">
-        <f t="shared" si="0"/>
+      <c r="J6">
+        <f t="array" ref="J6">COUNTIFS($G$2:$G$57,I6,$H$2:$H$57,"")</f>
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>17</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E7" s="3" t="s">
+      <c r="C7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" t="s">
         <v>11</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G7" s="3">
         <v>2320852</v>
       </c>
       <c r="H7" s="3"/>
-      <c r="J7" s="8">
-        <f t="array" ref="J7">INDEX($G$2:$G$52, MATCH(0, COUNTIF($J$1:J6, $G$2:$G$52), 0))</f>
+      <c r="I7" s="7">
+        <f t="array" ref="I7">INDEX($G$2:$G$56, MATCH(0, COUNTIF(I$1:$J6, $G$2:$G$56), 0))</f>
         <v>1438441</v>
       </c>
-      <c r="K7">
-        <f t="shared" si="0"/>
+      <c r="J7">
+        <f t="array" ref="J7">COUNTIFS($G$2:$G$57,I7,$H$2:$H$57,"")</f>
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>18</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E8" s="3" t="s">
+      <c r="C8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" t="s">
         <v>11</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G8" s="2">
         <v>1759265</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="J8" s="8">
-        <f t="array" ref="J8">INDEX($G$2:$G$52, MATCH(0, COUNTIF($J$1:J7, $G$2:$G$52), 0))</f>
+        <v>103</v>
+      </c>
+      <c r="I8" s="7">
+        <f t="array" ref="I8">INDEX($G$2:$G$56, MATCH(0, COUNTIF(I$1:$J7, $G$2:$G$56), 0))</f>
         <v>2336831</v>
       </c>
-      <c r="K8">
-        <f t="shared" si="0"/>
+      <c r="J8">
+        <f t="array" ref="J8">COUNTIFS($G$2:$G$57,I8,$H$2:$H$57,"")</f>
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>20</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E9" s="3" t="s">
+      <c r="C9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" t="s">
         <v>11</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G9" s="2">
         <v>1759265</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="J9" s="8">
-        <f t="array" ref="J9">INDEX($G$2:$G$52, MATCH(0, COUNTIF($J$1:J8, $G$2:$G$52), 0))</f>
+        <v>103</v>
+      </c>
+      <c r="I9" s="7">
+        <f t="array" ref="I9">INDEX($G$2:$G$56, MATCH(0, COUNTIF(I$1:$J8, $G$2:$G$56), 0))</f>
         <v>2336780</v>
       </c>
-      <c r="K9">
-        <f t="shared" si="0"/>
+      <c r="J9">
+        <f t="array" ref="J9">COUNTIFS($G$2:$G$57,I9,$H$2:$H$57,"")</f>
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>21</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E10" s="3" t="s">
+      <c r="C10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" t="s">
         <v>11</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G10" s="2">
         <v>1759265</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="J10" s="8">
-        <f t="array" ref="J10">INDEX($G$2:$G$52, MATCH(0, COUNTIF($J$1:J9, $G$2:$G$52), 0))</f>
+        <v>103</v>
+      </c>
+      <c r="I10" s="7">
+        <f t="array" ref="I10">INDEX($G$2:$G$56, MATCH(0, COUNTIF(I$1:$J9, $G$2:$G$56), 0))</f>
         <v>2352451</v>
       </c>
-      <c r="K10">
-        <f t="shared" si="0"/>
+      <c r="J10">
+        <f t="array" ref="J10">COUNTIFS($G$2:$G$57,I10,$H$2:$H$57,"")</f>
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>22</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C11" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E11" s="3" t="s">
+      <c r="C11" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11" t="s">
         <v>11</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G11" s="2">
         <v>1759265</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="J11" s="8">
-        <f t="array" ref="J11">INDEX($G$2:$G$52, MATCH(0, COUNTIF($J$1:J10, $G$2:$G$52), 0))</f>
+        <v>103</v>
+      </c>
+      <c r="I11" s="7">
+        <f t="array" ref="I11">INDEX($G$2:$G$56, MATCH(0, COUNTIF(I$1:$J10, $G$2:$G$56), 0))</f>
         <v>2129074</v>
       </c>
-      <c r="K11">
-        <f t="shared" si="0"/>
+      <c r="J11">
+        <f t="array" ref="J11">COUNTIFS($G$2:$G$57,I11,$H$2:$H$57,"")</f>
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>23</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C12" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E12" s="3" t="s">
+      <c r="C12" t="s">
+        <v>9</v>
+      </c>
+      <c r="D12" t="s">
+        <v>10</v>
+      </c>
+      <c r="E12" t="s">
         <v>11</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G12" s="2">
         <v>1759265</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="J12" s="8">
-        <f t="array" ref="J12">INDEX($G$2:$G$52, MATCH(0, COUNTIF($J$1:J11, $G$2:$G$52), 0))</f>
+        <v>103</v>
+      </c>
+      <c r="I12" s="7">
+        <f t="array" ref="I12">INDEX($G$2:$G$56, MATCH(0, COUNTIF(I$1:$J11, $G$2:$G$56), 0))</f>
         <v>9332391</v>
       </c>
-      <c r="K12">
-        <f t="shared" si="0"/>
+      <c r="J12">
+        <f t="array" ref="J12">COUNTIFS($G$2:$G$57,I12,$H$2:$H$57,"")</f>
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>24</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E13" s="3" t="s">
+      <c r="C13" t="s">
+        <v>9</v>
+      </c>
+      <c r="D13" t="s">
+        <v>10</v>
+      </c>
+      <c r="E13" t="s">
         <v>11</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G13" s="3">
         <v>2320852</v>
       </c>
       <c r="H13" s="3"/>
-      <c r="J13" s="8">
-        <f t="array" ref="J13">INDEX($G$2:$G$52, MATCH(0, COUNTIF($J$1:J12, $G$2:$G$52), 0))</f>
+      <c r="I13" s="7">
+        <f t="array" ref="I13">INDEX($G$2:$G$56, MATCH(0, COUNTIF(I$1:$J12, $G$2:$G$56), 0))</f>
         <v>2129087</v>
       </c>
-      <c r="K13">
-        <f t="shared" si="0"/>
+      <c r="J13">
+        <f t="array" ref="J13">COUNTIFS($G$2:$G$57,I13,$H$2:$H$57,"")</f>
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>25</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C14" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E14" s="3" t="s">
+      <c r="C14" t="s">
+        <v>9</v>
+      </c>
+      <c r="D14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E14" t="s">
         <v>11</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G14" s="2">
         <v>1759265</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="J14" s="8">
-        <f t="array" ref="J14">INDEX($G$2:$G$52, MATCH(0, COUNTIF($J$1:J13, $G$2:$G$52), 0))</f>
+        <v>103</v>
+      </c>
+      <c r="I14" s="7">
+        <f t="array" ref="I14">INDEX($G$2:$G$56, MATCH(0, COUNTIF(I$1:$J13, $G$2:$G$56), 0))</f>
         <v>2129237</v>
       </c>
-      <c r="K14">
-        <f t="shared" si="0"/>
+      <c r="J14">
+        <f t="array" ref="J14">COUNTIFS($G$2:$G$57,I14,$H$2:$H$57,"")</f>
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>26</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C15" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E15" s="3" t="s">
+      <c r="C15" t="s">
+        <v>9</v>
+      </c>
+      <c r="D15" t="s">
+        <v>10</v>
+      </c>
+      <c r="E15" t="s">
         <v>11</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G15" s="3">
         <v>2320852</v>
       </c>
       <c r="H15" s="3"/>
-      <c r="J15" s="8">
-        <f t="array" ref="J15">INDEX($G$2:$G$52, MATCH(0, COUNTIF($J$1:J14, $G$2:$G$52), 0))</f>
+      <c r="I15" s="7">
+        <f t="array" ref="I15">INDEX($G$2:$G$56, MATCH(0, COUNTIF(I$1:$J14, $G$2:$G$56), 0))</f>
         <v>2129171</v>
       </c>
-      <c r="K15">
-        <f t="shared" si="0"/>
+      <c r="J15">
+        <f t="array" ref="J15">COUNTIFS($G$2:$G$57,I15,$H$2:$H$57,"")</f>
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>27</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C16" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E16" s="3" t="s">
+      <c r="C16" t="s">
+        <v>9</v>
+      </c>
+      <c r="D16" t="s">
+        <v>10</v>
+      </c>
+      <c r="E16" t="s">
         <v>11</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G16" s="3">
         <v>2320852</v>
       </c>
       <c r="H16" s="3"/>
-      <c r="J16" s="8">
-        <f t="array" ref="J16">INDEX($G$2:$G$52, MATCH(0, COUNTIF($J$1:J15, $G$2:$G$52), 0))</f>
+      <c r="I16" s="7">
+        <f t="array" ref="I16">INDEX($G$2:$G$56, MATCH(0, COUNTIF(I$1:$J15, $G$2:$G$56), 0))</f>
         <v>2129150</v>
       </c>
-      <c r="K16">
-        <f t="shared" si="0"/>
+      <c r="J16">
+        <f t="array" ref="J16">COUNTIFS($G$2:$G$57,I16,$H$2:$H$57,"")</f>
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>28</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C17" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E17" s="3" t="s">
+      <c r="C17" t="s">
+        <v>9</v>
+      </c>
+      <c r="D17" t="s">
+        <v>10</v>
+      </c>
+      <c r="E17" t="s">
         <v>11</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G17" s="2">
         <v>1759265</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="J17" s="8">
-        <f t="array" ref="J17">INDEX($G$2:$G$52, MATCH(0, COUNTIF($J$1:J16, $G$2:$G$52), 0))</f>
+        <v>103</v>
+      </c>
+      <c r="I17" s="7">
+        <f t="array" ref="I17">INDEX($G$2:$G$56, MATCH(0, COUNTIF(I$1:$J16, $G$2:$G$56), 0))</f>
         <v>1838922</v>
       </c>
-      <c r="K17">
-        <f t="shared" si="0"/>
+      <c r="J17">
+        <f t="array" ref="J17">COUNTIFS($G$2:$G$57,I17,$H$2:$H$57,"")</f>
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>29</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C18" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E18" s="3" t="s">
+      <c r="C18" t="s">
+        <v>9</v>
+      </c>
+      <c r="D18" t="s">
+        <v>10</v>
+      </c>
+      <c r="E18" t="s">
         <v>11</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G18" s="2">
         <v>2320827</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="J18" s="8">
-        <f t="array" ref="J18">INDEX($G$2:$G$52, MATCH(0, COUNTIF($J$1:J17, $G$2:$G$52), 0))</f>
+        <v>103</v>
+      </c>
+      <c r="I18" s="7">
+        <f t="array" ref="I18">INDEX($G$2:$G$56, MATCH(0, COUNTIF(I$1:$J17, $G$2:$G$56), 0))</f>
         <v>9425586</v>
       </c>
-      <c r="K18">
-        <f t="shared" si="0"/>
+      <c r="J18">
+        <f t="array" ref="J18">COUNTIFS($G$2:$G$57,I18,$H$2:$H$57,"")</f>
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>31</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C19" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E19" s="3" t="s">
+      <c r="C19" t="s">
+        <v>9</v>
+      </c>
+      <c r="D19" t="s">
+        <v>10</v>
+      </c>
+      <c r="E19" t="s">
         <v>11</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G19" s="2">
         <v>1759265</v>
       </c>
       <c r="H19" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="J19" s="8">
-        <f t="array" ref="J19">INDEX($G$2:$G$52, MATCH(0, COUNTIF($J$1:J18, $G$2:$G$52), 0))</f>
+        <v>103</v>
+      </c>
+      <c r="I19" s="7">
+        <f t="array" ref="I19">INDEX($G$2:$G$56, MATCH(0, COUNTIF(I$1:$J18, $G$2:$G$56), 0))</f>
         <v>2102522</v>
       </c>
-      <c r="K19">
-        <f t="shared" si="0"/>
+      <c r="J19">
+        <f t="array" ref="J19">COUNTIFS($G$2:$G$57,I19,$H$2:$H$57,"")</f>
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>32</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C20" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E20" s="3" t="s">
+      <c r="C20" t="s">
+        <v>9</v>
+      </c>
+      <c r="D20" t="s">
+        <v>10</v>
+      </c>
+      <c r="E20" t="s">
         <v>11</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G20" s="2">
         <v>1759265</v>
       </c>
       <c r="H20" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="J20" s="8">
-        <f t="array" ref="J20">INDEX($G$2:$G$52, MATCH(0, COUNTIF($J$1:J19, $G$2:$G$52), 0))</f>
+        <v>103</v>
+      </c>
+      <c r="I20" s="7">
+        <f t="array" ref="I20">INDEX($G$2:$G$56, MATCH(0, COUNTIF(I$1:$J19, $G$2:$G$56), 0))</f>
         <v>2067770</v>
       </c>
-      <c r="K20">
-        <f t="shared" si="0"/>
+      <c r="J20">
+        <f t="array" ref="J20">COUNTIFS($G$2:$G$57,I20,$H$2:$H$57,"")</f>
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>33</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C21" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E21" s="3" t="s">
+      <c r="C21" t="s">
+        <v>9</v>
+      </c>
+      <c r="D21" t="s">
+        <v>10</v>
+      </c>
+      <c r="E21" t="s">
         <v>11</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G21" s="2">
         <v>2320827</v>
       </c>
       <c r="H21" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="J21" s="8" t="e">
-        <f t="array" ref="J21">INDEX($G$2:$G$52, MATCH(0, COUNTIF($J$1:J20, $G$2:$G$52), 0))</f>
+        <v>103</v>
+      </c>
+      <c r="I21" s="7" t="e">
+        <f t="array" ref="I21">INDEX($G$2:$G$56, MATCH(0, COUNTIF(I$1:$J20, $G$2:$G$56), 0))</f>
         <v>#N/A</v>
       </c>
-      <c r="K21">
-        <f t="shared" si="0"/>
+      <c r="J21">
+        <f t="array" ref="J21">COUNTIFS($G$2:$G$57,I21,$H$2:$H$57,"")</f>
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="3" t="s">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>34</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C22" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E22" s="3" t="s">
+      <c r="C22" t="s">
+        <v>9</v>
+      </c>
+      <c r="D22" t="s">
+        <v>10</v>
+      </c>
+      <c r="E22" t="s">
         <v>11</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G22" s="3">
         <v>2320852</v>
       </c>
       <c r="H22" s="3"/>
-      <c r="J22" s="8" t="e">
-        <f t="array" ref="J22">INDEX($G$2:$G$52, MATCH(0, COUNTIF($J$1:J21, $G$2:$G$52), 0))</f>
+      <c r="I22" s="7" t="e">
+        <f t="array" ref="I22">INDEX($G$2:$G$56, MATCH(0, COUNTIF(I$1:$J21, $G$2:$G$56), 0))</f>
         <v>#N/A</v>
       </c>
-      <c r="K22">
-        <f t="shared" si="0"/>
+      <c r="J22">
+        <f t="array" ref="J22">COUNTIFS($G$2:$G$57,I22,$H$2:$H$57,"")</f>
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="3" t="s">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>35</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C23" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E23" s="3" t="s">
+      <c r="C23" t="s">
+        <v>9</v>
+      </c>
+      <c r="D23" t="s">
+        <v>10</v>
+      </c>
+      <c r="E23" t="s">
         <v>11</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G23" s="2">
         <v>1759265</v>
       </c>
       <c r="H23" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="J23" s="8" t="e">
-        <f t="array" ref="J23">INDEX($G$2:$G$52, MATCH(0, COUNTIF($J$1:J22, $G$2:$G$52), 0))</f>
+        <v>103</v>
+      </c>
+      <c r="I23" s="7" t="e">
+        <f t="array" ref="I23">INDEX($G$2:$G$56, MATCH(0, COUNTIF(I$1:$J22, $G$2:$G$56), 0))</f>
         <v>#N/A</v>
       </c>
-      <c r="K23">
-        <f t="shared" si="0"/>
+      <c r="J23">
+        <f t="array" ref="J23">COUNTIFS($G$2:$G$57,I23,$H$2:$H$57,"")</f>
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="3" t="s">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>36</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C24" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D24" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E24" s="3" t="s">
+      <c r="C24" t="s">
+        <v>9</v>
+      </c>
+      <c r="D24" t="s">
+        <v>10</v>
+      </c>
+      <c r="E24" t="s">
         <v>11</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G24" s="2">
         <v>1759265</v>
       </c>
       <c r="H24" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="J24" s="8" t="e">
-        <f t="array" ref="J24">INDEX($G$2:$G$52, MATCH(0, COUNTIF($J$1:J23, $G$2:$G$52), 0))</f>
+        <v>103</v>
+      </c>
+      <c r="I24" s="7" t="e">
+        <f t="array" ref="I24">INDEX($G$2:$G$56, MATCH(0, COUNTIF(I$1:$J23, $G$2:$G$56), 0))</f>
         <v>#N/A</v>
       </c>
-      <c r="K24">
-        <f t="shared" si="0"/>
+      <c r="J24">
+        <f t="array" ref="J24">COUNTIFS($G$2:$G$57,I24,$H$2:$H$57,"")</f>
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" s="3" t="s">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>37</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C25" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D25" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E25" s="3" t="s">
+      <c r="C25" t="s">
+        <v>9</v>
+      </c>
+      <c r="D25" t="s">
+        <v>10</v>
+      </c>
+      <c r="E25" t="s">
         <v>11</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G25" s="3">
         <v>2320852</v>
       </c>
       <c r="H25" s="3"/>
-      <c r="J25" s="8" t="e">
-        <f t="array" ref="J25">INDEX($G$2:$G$52, MATCH(0, COUNTIF($J$1:J24, $G$2:$G$52), 0))</f>
+      <c r="I25" s="7" t="e">
+        <f t="array" ref="I25">INDEX($G$2:$G$56, MATCH(0, COUNTIF(I$1:$J24, $G$2:$G$56), 0))</f>
         <v>#N/A</v>
       </c>
-      <c r="K25">
-        <f t="shared" si="0"/>
+      <c r="J25">
+        <f t="array" ref="J25">COUNTIFS($G$2:$G$57,I25,$H$2:$H$57,"")</f>
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" s="3" t="s">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>38</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C26" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E26" s="3" t="s">
+      <c r="C26" t="s">
+        <v>9</v>
+      </c>
+      <c r="D26" t="s">
+        <v>10</v>
+      </c>
+      <c r="E26" t="s">
         <v>11</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G26" s="2">
         <v>1759265</v>
       </c>
       <c r="H26" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="J26" s="8" t="e">
-        <f t="array" ref="J26">INDEX($G$2:$G$52, MATCH(0, COUNTIF($J$1:J25, $G$2:$G$52), 0))</f>
+        <v>103</v>
+      </c>
+      <c r="I26" s="7" t="e">
+        <f t="array" ref="I26">INDEX($G$2:$G$56, MATCH(0, COUNTIF(I$1:$J25, $G$2:$G$56), 0))</f>
         <v>#N/A</v>
       </c>
-      <c r="K26">
-        <f t="shared" si="0"/>
+      <c r="J26">
+        <f t="array" ref="J26">COUNTIFS($G$2:$G$57,I26,$H$2:$H$57,"")</f>
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" s="3" t="s">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>39</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C27" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D27" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E27" s="3" t="s">
+      <c r="C27" t="s">
+        <v>9</v>
+      </c>
+      <c r="D27" t="s">
+        <v>10</v>
+      </c>
+      <c r="E27" t="s">
         <v>11</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G27" s="2">
         <v>1759246</v>
       </c>
       <c r="H27" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="J27" s="8" t="e">
-        <f t="array" ref="J27">INDEX($G$2:$G$52, MATCH(0, COUNTIF($J$1:J26, $G$2:$G$52), 0))</f>
+        <v>103</v>
+      </c>
+      <c r="I27" s="7" t="e">
+        <f t="array" ref="I27">INDEX($G$2:$G$56, MATCH(0, COUNTIF(I$1:$J26, $G$2:$G$56), 0))</f>
         <v>#N/A</v>
       </c>
-      <c r="K27">
-        <f t="shared" si="0"/>
+      <c r="J27">
+        <f t="array" ref="J27">COUNTIFS($G$2:$G$57,I27,$H$2:$H$57,"")</f>
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" s="3" t="s">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>40</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C28" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D28" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E28" s="3" t="s">
+      <c r="C28" t="s">
+        <v>9</v>
+      </c>
+      <c r="D28" t="s">
+        <v>10</v>
+      </c>
+      <c r="E28" t="s">
         <v>11</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G28" s="2">
         <v>2320827</v>
       </c>
       <c r="H28" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="J28" s="8" t="e">
-        <f t="array" ref="J28">INDEX($G$2:$G$52, MATCH(0, COUNTIF($J$1:J27, $G$2:$G$52), 0))</f>
+        <v>103</v>
+      </c>
+      <c r="I28" s="7" t="e">
+        <f t="array" ref="I28">INDEX($G$2:$G$56, MATCH(0, COUNTIF(I$1:$J27, $G$2:$G$56), 0))</f>
         <v>#N/A</v>
       </c>
-      <c r="K28">
-        <f t="shared" si="0"/>
+      <c r="J28">
+        <f t="array" ref="J28">COUNTIFS($G$2:$G$57,I28,$H$2:$H$57,"")</f>
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" s="3" t="s">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>41</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C29" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D29" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E29" s="3" t="s">
+      <c r="C29" t="s">
+        <v>9</v>
+      </c>
+      <c r="D29" t="s">
+        <v>10</v>
+      </c>
+      <c r="E29" t="s">
         <v>11</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G29" s="3">
         <v>2320852</v>
       </c>
       <c r="H29" s="3"/>
-      <c r="J29" s="8" t="e">
-        <f t="array" ref="J29">INDEX($G$2:$G$52, MATCH(0, COUNTIF($J$1:J28, $G$2:$G$52), 0))</f>
+      <c r="I29" s="7" t="e">
+        <f t="array" ref="I29">INDEX($G$2:$G$56, MATCH(0, COUNTIF(I$1:$J28, $G$2:$G$56), 0))</f>
         <v>#N/A</v>
       </c>
-      <c r="K29">
-        <f t="shared" si="0"/>
+      <c r="J29">
+        <f t="array" ref="J29">COUNTIFS($G$2:$G$57,I29,$H$2:$H$57,"")</f>
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A30" s="3" t="s">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>42</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C30" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D30" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E30" s="3" t="s">
+      <c r="C30" t="s">
+        <v>9</v>
+      </c>
+      <c r="D30" t="s">
+        <v>10</v>
+      </c>
+      <c r="E30" t="s">
         <v>11</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G30" s="2">
         <v>1759265</v>
       </c>
       <c r="H30" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="J30" s="8" t="e">
-        <f t="array" ref="J30">INDEX($G$2:$G$52, MATCH(0, COUNTIF($J$1:J29, $G$2:$G$52), 0))</f>
+        <v>103</v>
+      </c>
+      <c r="I30" s="7" t="e">
+        <f t="array" ref="I30">INDEX($G$2:$G$56, MATCH(0, COUNTIF(I$1:$J29, $G$2:$G$56), 0))</f>
         <v>#N/A</v>
       </c>
-      <c r="K30">
-        <f t="shared" si="0"/>
+      <c r="J30">
+        <f t="array" ref="J30">COUNTIFS($G$2:$G$57,I30,$H$2:$H$57,"")</f>
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A31" s="3" t="s">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
         <v>43</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C31" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D31" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E31" s="3" t="s">
+      <c r="C31" t="s">
+        <v>9</v>
+      </c>
+      <c r="D31" t="s">
+        <v>10</v>
+      </c>
+      <c r="E31" t="s">
         <v>11</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G31" s="2">
         <v>2320827</v>
       </c>
       <c r="H31" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="J31" s="8" t="e">
-        <f t="array" ref="J31">INDEX($G$2:$G$52, MATCH(0, COUNTIF($J$1:J30, $G$2:$G$52), 0))</f>
+        <v>103</v>
+      </c>
+      <c r="I31" s="7" t="e">
+        <f t="array" ref="I31">INDEX($G$2:$G$56, MATCH(0, COUNTIF(I$1:$J30, $G$2:$G$56), 0))</f>
         <v>#N/A</v>
       </c>
-      <c r="K31">
-        <f t="shared" si="0"/>
+      <c r="J31">
+        <f t="array" ref="J31">COUNTIFS($G$2:$G$57,I31,$H$2:$H$57,"")</f>
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A32" s="3" t="s">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>44</v>
       </c>
       <c r="B32" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C32" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D32" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E32" s="3" t="s">
+      <c r="C32" t="s">
+        <v>9</v>
+      </c>
+      <c r="D32" t="s">
+        <v>10</v>
+      </c>
+      <c r="E32" t="s">
         <v>11</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G32" s="3">
         <v>2320852</v>
       </c>
       <c r="H32" s="3"/>
-      <c r="J32" s="8" t="e">
-        <f t="array" ref="J32">INDEX($G$2:$G$52, MATCH(0, COUNTIF($J$1:J31, $G$2:$G$52), 0))</f>
+      <c r="I32" s="7" t="e">
+        <f t="array" ref="I32">INDEX($G$2:$G$56, MATCH(0, COUNTIF(I$1:$J31, $G$2:$G$56), 0))</f>
         <v>#N/A</v>
       </c>
+      <c r="J32">
+        <f t="array" ref="J32">COUNTIFS($G$2:$G$57,I32,$H$2:$H$57,"")</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A33" s="3" t="s">
+      <c r="A33" t="s">
         <v>45</v>
       </c>
       <c r="B33" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C33" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D33" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E33" s="3" t="s">
+      <c r="C33" t="s">
+        <v>9</v>
+      </c>
+      <c r="D33" t="s">
+        <v>10</v>
+      </c>
+      <c r="E33" t="s">
         <v>11</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G33" s="2">
         <v>1759265</v>
       </c>
       <c r="H33" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="J33" s="8" t="e">
-        <f t="array" ref="J33">INDEX($G$2:$G$52, MATCH(0, COUNTIF($J$1:J32, $G$2:$G$52), 0))</f>
+        <v>103</v>
+      </c>
+      <c r="I33" s="7" t="e">
+        <f t="array" ref="I33">INDEX($G$2:$G$56, MATCH(0, COUNTIF(I$1:$J32, $G$2:$G$56), 0))</f>
         <v>#N/A</v>
       </c>
+      <c r="J33">
+        <f t="array" ref="J33">COUNTIFS($G$2:$G$57,I33,$H$2:$H$57,"")</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A34" s="3" t="s">
+      <c r="A34" t="s">
         <v>46</v>
       </c>
       <c r="B34" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C34" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D34" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E34" s="3" t="s">
+      <c r="C34" t="s">
+        <v>9</v>
+      </c>
+      <c r="D34" t="s">
+        <v>10</v>
+      </c>
+      <c r="E34" t="s">
         <v>11</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G34" s="2">
         <v>2320827</v>
       </c>
       <c r="H34" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="J34" s="8" t="e">
-        <f t="array" ref="J34">INDEX($G$2:$G$52, MATCH(0, COUNTIF($J$1:J33, $G$2:$G$52), 0))</f>
+        <v>103</v>
+      </c>
+      <c r="I34" s="7" t="e">
+        <f t="array" ref="I34">INDEX($G$2:$G$56, MATCH(0, COUNTIF(I$1:$J33, $G$2:$G$56), 0))</f>
         <v>#N/A</v>
       </c>
+      <c r="J34">
+        <f t="array" ref="J34">COUNTIFS($G$2:$G$57,I34,$H$2:$H$57,"")</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A35" s="3" t="s">
+      <c r="A35" t="s">
         <v>47</v>
       </c>
       <c r="B35" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C35" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D35" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E35" s="3" t="s">
+      <c r="C35" t="s">
+        <v>9</v>
+      </c>
+      <c r="D35" t="s">
+        <v>10</v>
+      </c>
+      <c r="E35" t="s">
         <v>11</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G35" s="2">
         <v>1759265</v>
       </c>
       <c r="H35" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="J35" s="8" t="e">
-        <f t="array" ref="J35">INDEX($G$2:$G$52, MATCH(0, COUNTIF($J$1:J34, $G$2:$G$52), 0))</f>
+        <v>103</v>
+      </c>
+      <c r="I35" s="7" t="e">
+        <f t="array" ref="I35">INDEX($G$2:$G$56, MATCH(0, COUNTIF(I$1:$J34, $G$2:$G$56), 0))</f>
         <v>#N/A</v>
       </c>
+      <c r="J35">
+        <f t="array" ref="J35">COUNTIFS($G$2:$G$57,I35,$H$2:$H$57,"")</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A36" s="3" t="s">
+      <c r="A36" t="s">
         <v>48</v>
       </c>
-      <c r="B36" s="3" t="s">
+      <c r="B36" t="s">
         <v>49</v>
       </c>
-      <c r="C36" s="3" t="s">
+      <c r="C36" t="s">
         <v>49</v>
       </c>
-      <c r="D36" s="3" t="s">
+      <c r="D36" t="s">
+        <v>118</v>
+      </c>
+      <c r="E36" t="s">
+        <v>50</v>
+      </c>
+      <c r="F36" s="2" t="s">
         <v>100</v>
-      </c>
-      <c r="E36" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="F36" s="2" t="s">
-        <v>101</v>
       </c>
       <c r="G36" s="2">
         <v>2102587</v>
       </c>
       <c r="H36" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="J36" s="8" t="e">
-        <f t="array" ref="J36">INDEX($G$2:$G$52, MATCH(0, COUNTIF($J$1:J35, $G$2:$G$52), 0))</f>
+        <v>103</v>
+      </c>
+      <c r="I36" s="7" t="e">
+        <f t="array" ref="I36">INDEX($G$2:$G$56, MATCH(0, COUNTIF(I$1:$J35, $G$2:$G$56), 0))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A37" s="3" t="s">
+      <c r="A37" t="s">
         <v>51</v>
       </c>
-      <c r="B37" s="3" t="s">
+      <c r="B37" t="s">
         <v>52</v>
       </c>
-      <c r="C37" s="3" t="s">
+      <c r="C37" t="s">
         <v>52</v>
       </c>
-      <c r="D37" s="3" t="s">
+      <c r="D37" t="s">
         <v>53</v>
       </c>
-      <c r="E37" s="3" t="s">
+      <c r="E37" t="s">
         <v>54</v>
       </c>
       <c r="F37" s="3" t="s">
@@ -2512,25 +2536,25 @@
         <v>1438441</v>
       </c>
       <c r="H37" s="3"/>
-      <c r="J37" s="8" t="e">
-        <f t="array" ref="J37">INDEX($G$2:$G$52, MATCH(0, COUNTIF($J$1:J36, $G$2:$G$52), 0))</f>
+      <c r="I37" s="7" t="e">
+        <f t="array" ref="I37">INDEX($G$2:$G$56, MATCH(0, COUNTIF(I$1:$J36, $G$2:$G$56), 0))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A38" s="3" t="s">
+      <c r="A38" t="s">
         <v>56</v>
       </c>
-      <c r="B38" s="3" t="s">
+      <c r="B38" t="s">
         <v>57</v>
       </c>
-      <c r="C38" s="3" t="s">
+      <c r="C38" t="s">
         <v>58</v>
       </c>
-      <c r="D38" s="3" t="s">
+      <c r="D38" t="s">
         <v>59</v>
       </c>
-      <c r="E38" s="3" t="s">
+      <c r="E38" t="s">
         <v>60</v>
       </c>
       <c r="F38" s="2" t="s">
@@ -2540,57 +2564,57 @@
         <v>2336831</v>
       </c>
       <c r="H38" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="J38" s="8" t="e">
-        <f t="array" ref="J38">INDEX($G$2:$G$52, MATCH(0, COUNTIF($J$1:J37, $G$2:$G$52), 0))</f>
+        <v>103</v>
+      </c>
+      <c r="I38" s="7" t="e">
+        <f t="array" ref="I38">INDEX($G$2:$G$52, MATCH(0, COUNTIF(I$1:$J37, $G$2:$G$52), 0))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A39" s="3" t="s">
+      <c r="A39" t="s">
         <v>61</v>
       </c>
-      <c r="B39" s="3" t="s">
+      <c r="B39" t="s">
         <v>62</v>
       </c>
-      <c r="C39" s="3" t="s">
+      <c r="C39" t="s">
         <v>63</v>
       </c>
-      <c r="D39" s="3" t="s">
+      <c r="D39" t="s">
         <v>64</v>
       </c>
-      <c r="E39" s="3" t="s">
+      <c r="E39" t="s">
         <v>65</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G39" s="2">
         <v>2336780</v>
       </c>
       <c r="H39" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="J39" s="8" t="e">
-        <f t="array" ref="J39">INDEX($G$2:$G$52, MATCH(0, COUNTIF($J$1:J38, $G$2:$G$52), 0))</f>
+        <v>103</v>
+      </c>
+      <c r="I39" s="7" t="e">
+        <f t="array" ref="I39">INDEX($G$2:$G$52, MATCH(0, COUNTIF(I$1:$J38, $G$2:$G$52), 0))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A40" s="3" t="s">
+      <c r="A40" t="s">
         <v>66</v>
       </c>
-      <c r="B40" s="3" t="s">
+      <c r="B40" t="s">
         <v>67</v>
       </c>
-      <c r="C40" s="3" t="s">
+      <c r="C40" t="s">
         <v>68</v>
       </c>
-      <c r="D40" s="3" t="s">
+      <c r="D40" t="s">
         <v>69</v>
       </c>
-      <c r="E40" s="3" t="s">
+      <c r="E40" t="s">
         <v>70</v>
       </c>
       <c r="F40" s="2" t="s">
@@ -2600,389 +2624,492 @@
         <v>2352451</v>
       </c>
       <c r="H40" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="J40" s="8" t="e">
-        <f t="array" ref="J40">INDEX($G$2:$G$52, MATCH(0, COUNTIF($J$1:J39, $G$2:$G$52), 0))</f>
+        <v>103</v>
+      </c>
+      <c r="I40" s="7" t="e">
+        <f t="array" ref="I40">INDEX($G$2:$G$52, MATCH(0, COUNTIF(I$1:$J39, $G$2:$G$52), 0))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A41" s="3" t="s">
+      <c r="A41" t="s">
         <v>71</v>
       </c>
-      <c r="B41" s="3">
+      <c r="B41">
         <v>330</v>
       </c>
-      <c r="C41" s="3" t="s">
+      <c r="C41" t="s">
         <v>72</v>
       </c>
-      <c r="D41" s="3" t="s">
+      <c r="D41" t="s">
         <v>73</v>
       </c>
-      <c r="E41" s="3" t="s">
+      <c r="E41" t="s">
         <v>74</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G41" s="2">
         <v>2129074</v>
       </c>
       <c r="H41" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="J41" s="8" t="e">
-        <f t="array" ref="J41">INDEX($G$2:$G$52, MATCH(0, COUNTIF($J$1:J40, $G$2:$G$52), 0))</f>
+        <v>103</v>
+      </c>
+      <c r="I41" s="7" t="e">
+        <f t="array" ref="I41">INDEX($G$2:$G$52, MATCH(0, COUNTIF(I$1:$J40, $G$2:$G$52), 0))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A42" s="3" t="s">
+      <c r="A42" t="s">
         <v>75</v>
       </c>
-      <c r="B42" s="3" t="s">
+      <c r="B42" t="s">
         <v>76</v>
       </c>
-      <c r="C42" s="3" t="s">
+      <c r="C42" t="s">
         <v>72</v>
       </c>
-      <c r="D42" s="3" t="s">
+      <c r="D42" t="s">
         <v>73</v>
       </c>
-      <c r="E42" s="3" t="s">
+      <c r="E42" t="s">
         <v>74</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G42" s="2">
         <v>9332391</v>
       </c>
       <c r="H42" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="I42" s="7" t="e">
+        <f t="array" ref="I42">INDEX($G$2:$G$52, MATCH(0, COUNTIF(I$1:$J41, $G$2:$G$52), 0))</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>77</v>
+      </c>
+      <c r="B43">
+        <v>470</v>
+      </c>
+      <c r="C43" t="s">
+        <v>72</v>
+      </c>
+      <c r="D43" t="s">
+        <v>73</v>
+      </c>
+      <c r="E43" t="s">
+        <v>74</v>
+      </c>
+      <c r="F43" s="2" t="s">
         <v>104</v>
-      </c>
-      <c r="J42" s="8" t="e">
-        <f t="array" ref="J42">INDEX($G$2:$G$52, MATCH(0, COUNTIF($J$1:J41, $G$2:$G$52), 0))</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A43" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="B43" s="3">
-        <v>470</v>
-      </c>
-      <c r="C43" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="D43" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="E43" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="F43" s="2" t="s">
-        <v>105</v>
       </c>
       <c r="G43" s="2">
         <v>2129087</v>
       </c>
       <c r="H43" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="J43" s="8" t="e">
-        <f t="array" ref="J43">INDEX($G$2:$G$52, MATCH(0, COUNTIF($J$1:J42, $G$2:$G$52), 0))</f>
+        <v>103</v>
+      </c>
+      <c r="I43" s="7" t="e">
+        <f t="array" ref="I43">INDEX($G$2:$G$52, MATCH(0, COUNTIF(I$1:$J42, $G$2:$G$52), 0))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A44" s="3" t="s">
+      <c r="A44" t="s">
         <v>78</v>
       </c>
-      <c r="B44" s="3" t="s">
+      <c r="B44" t="s">
         <v>79</v>
       </c>
-      <c r="C44" s="3" t="s">
+      <c r="C44" t="s">
         <v>72</v>
       </c>
-      <c r="D44" s="3" t="s">
+      <c r="D44" t="s">
         <v>73</v>
       </c>
-      <c r="E44" s="3" t="s">
+      <c r="E44" t="s">
         <v>74</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G44" s="2">
         <v>2129237</v>
       </c>
       <c r="H44" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="J44" s="8" t="e">
-        <f t="array" ref="J44">INDEX($G$2:$G$52, MATCH(0, COUNTIF($J$1:J43, $G$2:$G$52), 0))</f>
+        <v>103</v>
+      </c>
+      <c r="I44" s="7" t="e">
+        <f t="array" ref="I44">INDEX($G$2:$G$52, MATCH(0, COUNTIF(I$1:$J43, $G$2:$G$52), 0))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A45" s="3" t="s">
+      <c r="A45" t="s">
         <v>80</v>
       </c>
-      <c r="B45" s="3" t="s">
+      <c r="B45" t="s">
         <v>76</v>
       </c>
-      <c r="C45" s="3" t="s">
+      <c r="C45" t="s">
         <v>72</v>
       </c>
-      <c r="D45" s="3" t="s">
+      <c r="D45" t="s">
         <v>73</v>
       </c>
-      <c r="E45" s="3" t="s">
+      <c r="E45" t="s">
         <v>74</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G45" s="2">
         <v>9332391</v>
       </c>
       <c r="H45" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="J45" s="8" t="e">
-        <f t="array" ref="J45">INDEX($G$2:$G$52, MATCH(0, COUNTIF($J$1:J44, $G$2:$G$52), 0))</f>
+        <v>103</v>
+      </c>
+      <c r="I45" s="7" t="e">
+        <f t="array" ref="I45">INDEX($G$2:$G$52, MATCH(0, COUNTIF(I$1:$J44, $G$2:$G$52), 0))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A46" s="3" t="s">
+      <c r="A46" t="s">
         <v>81</v>
       </c>
-      <c r="B46" s="3" t="s">
+      <c r="B46" t="s">
         <v>82</v>
       </c>
-      <c r="C46" s="3" t="s">
+      <c r="C46" t="s">
         <v>72</v>
       </c>
-      <c r="D46" s="3" t="s">
+      <c r="D46" t="s">
         <v>73</v>
       </c>
-      <c r="E46" s="3" t="s">
+      <c r="E46" t="s">
         <v>74</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G46" s="2">
         <v>2129171</v>
       </c>
       <c r="H46" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="J46" s="8" t="e">
-        <f t="array" ref="J46">INDEX($G$2:$G$52, MATCH(0, COUNTIF($J$1:J45, $G$2:$G$52), 0))</f>
+        <v>103</v>
+      </c>
+      <c r="I46" s="7" t="e">
+        <f t="array" ref="I46">INDEX($G$2:$G$52, MATCH(0, COUNTIF(I$1:$J45, $G$2:$G$52), 0))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A47" s="3" t="s">
+      <c r="A47" t="s">
         <v>83</v>
       </c>
-      <c r="B47" s="3" t="s">
+      <c r="B47" t="s">
         <v>84</v>
       </c>
-      <c r="C47" s="3" t="s">
+      <c r="C47" t="s">
         <v>72</v>
       </c>
-      <c r="D47" s="3" t="s">
+      <c r="D47" t="s">
         <v>73</v>
       </c>
-      <c r="E47" s="3" t="s">
+      <c r="E47" t="s">
         <v>74</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G47" s="2">
         <v>2129150</v>
       </c>
       <c r="H47" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="J47" s="8" t="e">
-        <f t="array" ref="J47">INDEX($G$2:$G$52, MATCH(0, COUNTIF($J$1:J46, $G$2:$G$52), 0))</f>
+        <v>103</v>
+      </c>
+      <c r="I47" s="7" t="e">
+        <f t="array" ref="I47">INDEX($G$2:$G$52, MATCH(0, COUNTIF(I$1:$J46, $G$2:$G$52), 0))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A48" s="3" t="s">
+      <c r="A48" t="s">
+        <v>119</v>
+      </c>
+      <c r="B48" t="s">
+        <v>76</v>
+      </c>
+      <c r="C48" t="s">
+        <v>72</v>
+      </c>
+      <c r="D48" t="s">
+        <v>73</v>
+      </c>
+      <c r="E48" t="s">
+        <v>74</v>
+      </c>
+      <c r="F48" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="G48" s="2">
+        <v>9332391</v>
+      </c>
+      <c r="H48" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="I48" s="7" t="e">
+        <f t="array" ref="I48">INDEX($G$2:$G$52, MATCH(0, COUNTIF(I$1:$J47, $G$2:$G$52), 0))</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>120</v>
+      </c>
+      <c r="B49" t="s">
+        <v>76</v>
+      </c>
+      <c r="C49" t="s">
+        <v>72</v>
+      </c>
+      <c r="D49" t="s">
+        <v>73</v>
+      </c>
+      <c r="E49" t="s">
+        <v>74</v>
+      </c>
+      <c r="F49" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="G49" s="2">
+        <v>9332391</v>
+      </c>
+      <c r="H49" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="I49" s="7" t="e">
+        <f t="array" ref="I49">INDEX($G$2:$G$52, MATCH(0, COUNTIF(I$1:$J48, $G$2:$G$52), 0))</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>121</v>
+      </c>
+      <c r="B50" t="s">
+        <v>76</v>
+      </c>
+      <c r="C50" t="s">
+        <v>72</v>
+      </c>
+      <c r="D50" t="s">
+        <v>73</v>
+      </c>
+      <c r="E50" t="s">
+        <v>74</v>
+      </c>
+      <c r="F50" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="G50" s="2">
+        <v>9332391</v>
+      </c>
+      <c r="H50" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>122</v>
+      </c>
+      <c r="B51" t="s">
+        <v>76</v>
+      </c>
+      <c r="C51" t="s">
+        <v>72</v>
+      </c>
+      <c r="D51" t="s">
+        <v>73</v>
+      </c>
+      <c r="E51" t="s">
+        <v>74</v>
+      </c>
+      <c r="F51" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="G51" s="2">
+        <v>9332391</v>
+      </c>
+      <c r="H51" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
         <v>85</v>
       </c>
-      <c r="B48" s="3" t="s">
+      <c r="B52" t="s">
         <v>86</v>
       </c>
-      <c r="C48" s="3" t="s">
+      <c r="C52" t="s">
         <v>86</v>
       </c>
-      <c r="D48" s="3" t="s">
+      <c r="D52" t="s">
         <v>87</v>
       </c>
-      <c r="E48" s="3" t="s">
+      <c r="E52" t="s">
         <v>88</v>
       </c>
-      <c r="F48" s="3" t="s">
+      <c r="F52" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="G48" s="3">
+      <c r="G52" s="3">
         <v>1838922</v>
       </c>
-      <c r="H48" s="3"/>
-      <c r="J48" s="8" t="e">
-        <f t="array" ref="J48">INDEX($G$2:$G$52, MATCH(0, COUNTIF($J$1:J47, $G$2:$G$52), 0))</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A49" s="3" t="s">
+      <c r="J52">
+        <f>SUM(J2:J35)</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
         <v>89</v>
       </c>
-      <c r="B49" s="3" t="s">
+      <c r="B53" t="s">
         <v>90</v>
       </c>
-      <c r="C49" s="3" t="s">
+      <c r="C53" t="s">
         <v>90</v>
       </c>
-      <c r="D49" s="3" t="s">
+      <c r="D53" t="s">
         <v>91</v>
       </c>
-      <c r="E49" s="3" t="s">
+      <c r="E53" t="s">
         <v>92</v>
       </c>
-      <c r="F49" s="3" t="s">
+      <c r="F53" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="G49" s="3">
+      <c r="G53" s="3">
         <v>9425586</v>
       </c>
-      <c r="H49" s="3"/>
-      <c r="J49" s="8" t="e">
-        <f t="array" ref="J49">INDEX($G$2:$G$52, MATCH(0, COUNTIF($J$1:J48, $G$2:$G$52), 0))</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A50" s="3" t="s">
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
         <v>93</v>
       </c>
-      <c r="B50" s="3" t="s">
+      <c r="B54" t="s">
         <v>94</v>
       </c>
-      <c r="C50" s="3" t="s">
+      <c r="C54" t="s">
         <v>94</v>
       </c>
-      <c r="D50" s="3" t="s">
+      <c r="D54" t="s">
         <v>87</v>
       </c>
-      <c r="E50" s="3" t="s">
+      <c r="E54" t="s">
         <v>95</v>
       </c>
-      <c r="F50" s="3" t="s">
+      <c r="F54" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="G50" s="6">
+      <c r="G54" s="5">
         <v>2102522</v>
       </c>
-      <c r="H50" s="3"/>
-    </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A51" s="3" t="s">
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
         <v>96</v>
       </c>
-      <c r="B51" s="3" t="s">
+      <c r="B55" t="s">
         <v>97</v>
       </c>
-      <c r="C51" s="3" t="s">
+      <c r="C55" t="s">
         <v>97</v>
       </c>
-      <c r="D51" s="3" t="s">
+      <c r="D55" t="s">
         <v>87</v>
       </c>
-      <c r="E51" s="3" t="s">
+      <c r="E55" t="s">
         <v>98</v>
       </c>
-      <c r="F51" s="3" t="s">
+      <c r="F55" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="G51" s="3">
+      <c r="G55" s="3">
         <v>2067770</v>
       </c>
-      <c r="H51" s="3"/>
-    </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A52" s="3" t="s">
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
         <v>99</v>
       </c>
-      <c r="B52" s="3" t="s">
+      <c r="B56" t="s">
         <v>97</v>
       </c>
-      <c r="C52" s="3" t="s">
+      <c r="C56" t="s">
         <v>97</v>
       </c>
-      <c r="D52" s="3" t="s">
+      <c r="D56" t="s">
         <v>87</v>
       </c>
-      <c r="E52" s="3" t="s">
+      <c r="E56" t="s">
         <v>98</v>
       </c>
-      <c r="F52" s="3" t="s">
+      <c r="F56" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="G52" s="3">
+      <c r="G56" s="3">
         <v>2067770</v>
       </c>
-      <c r="H52" s="3"/>
-    </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="F55" s="3" t="s">
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F59" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="G59" s="4">
+        <f t="array" ref="G59">SUM(1/COUNTIF(G2:G56,G2:G56))</f>
+        <v>18.999999999999996</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F60" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="G55" s="5">
-        <f t="array" ref="G55">SUM(1/COUNTIF(G2:G52,G2:G52))</f>
-        <v>19</v>
-      </c>
-    </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="F56" s="3" t="s">
+      <c r="G60" s="4">
+        <f t="array" ref="G60">COUNTIF(H2:H56,"PCB*")</f>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F61" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="G56" s="5">
-        <f>COUNTIF(H2:H52,"PCB*")</f>
-        <v>36</v>
-      </c>
-    </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="F57" s="3" t="s">
+      <c r="G61" s="4">
+        <f>COUNTBLANK(H2:H56)</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F62" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="G57" s="5">
-        <f>COUNTBLANK(H2:H52)</f>
-        <v>15</v>
-      </c>
-    </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="F58" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="G58" s="5">
-        <f>SUM(G56:G57)</f>
-        <v>51</v>
+      <c r="G62" s="4">
+        <f>SUM(G60:G61)</f>
+        <v>55</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="K1:K1048576">
+  <conditionalFormatting sqref="J2:J49">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>

</xml_diff>